<commit_message>
fix empty row height/cell width, #235
</commit_message>
<xml_diff>
--- a/tests/data/13_custom_heights_widths.xlsx
+++ b/tests/data/13_custom_heights_widths.xlsx
@@ -26,31 +26,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>170xd</t>
-  </si>
-  <si>
-    <t>40xd</t>
-  </si>
-  <si>
-    <t>dxd</t>
-  </si>
-  <si>
-    <t>dx30</t>
-  </si>
-  <si>
-    <t>170x30</t>
-  </si>
-  <si>
-    <t>40x30</t>
-  </si>
-  <si>
-    <t>170x10</t>
-  </si>
-  <si>
-    <t>40x10</t>
-  </si>
-  <si>
-    <t>dx10</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -365,49 +365,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
re-save custom_heights_widths.xlsx, add defaultColWidth sheet attribute
-- custom_heights was the only test sheet where the integral value was being saved with a trailing ".0"
-- Updated tests to expect the new values
-- added the new property "defaultColWidth"
</commit_message>
<xml_diff>
--- a/tests/data/13_custom_heights_widths.xlsx
+++ b/tests/data/13_custom_heights_widths.xlsx
@@ -366,7 +366,7 @@
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="100.0" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="100.0" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
@@ -400,7 +400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="100.0" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:4" ht="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>